<commit_message>
alerando algumas funcionalidade do product backlog
</commit_message>
<xml_diff>
--- a/backlog do produto.xlsx
+++ b/backlog do produto.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>BACKLOG DO PRODUTO</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Interface para interação c/o usuário</t>
+  </si>
+  <si>
+    <t>Área de histórico</t>
+  </si>
+  <si>
+    <t>Área de histórico de calculo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -192,6 +201,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -211,15 +229,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -523,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,149 +546,156 @@
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="11">
         <v>1</v>
       </c>
-      <c r="G2" s="18"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="11"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="14"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="11"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -688,7 +704,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G14" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do Backlog do Produto
</commit_message>
<xml_diff>
--- a/backlog do produto.xlsx
+++ b/backlog do produto.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="5205"/>
+    <workbookView xWindow="360" yWindow="72" windowWidth="14352" windowHeight="5208"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>BACKLOG DO PRODUTO</t>
   </si>
@@ -36,50 +36,56 @@
     <t>Calculadora_Ebeta</t>
   </si>
   <si>
-    <t>Somar</t>
-  </si>
-  <si>
-    <t>Subtrair</t>
-  </si>
-  <si>
-    <t>Dividir</t>
-  </si>
-  <si>
-    <t>Multiplicar</t>
-  </si>
-  <si>
     <t>Interface</t>
   </si>
   <si>
-    <t>Cria a funcionalidade de somar</t>
-  </si>
-  <si>
-    <t>Cria a funcionalidade de subtrair</t>
-  </si>
-  <si>
-    <t>Cria a funcionalidade de dividir</t>
-  </si>
-  <si>
-    <t>Cria a funcionalidade de multiplicar</t>
-  </si>
-  <si>
-    <t>Interface para interação c/o usuário</t>
-  </si>
-  <si>
     <t>Área de histórico</t>
   </si>
   <si>
-    <t>Área de histórico de calculo</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Conversor de Temperatura</t>
+  </si>
+  <si>
+    <t>Conversor de Ângulo</t>
+  </si>
+  <si>
+    <t>Construção do HTML</t>
+  </si>
+  <si>
+    <t>Criação de Tela</t>
+  </si>
+  <si>
+    <t>Criação do Estilo</t>
+  </si>
+  <si>
+    <t>Construção do CSS</t>
+  </si>
+  <si>
+    <t>Implementando Histórico</t>
+  </si>
+  <si>
+    <t>Criação de Script</t>
+  </si>
+  <si>
+    <t>Construção do JavaScript</t>
+  </si>
+  <si>
+    <t>Junção HTML ao CSS/ Intereção com o usuário</t>
+  </si>
+  <si>
+    <t>Implementação de um convesor de Temperatura</t>
+  </si>
+  <si>
+    <t>Implementação de um convesor de Ângulo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,11 +231,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -320,7 +335,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -355,7 +369,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -531,22 +544,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -557,7 +570,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -574,7 +587,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
@@ -587,94 +600,98 @@
       <c r="F3" s="12"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+        <v>14</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+        <v>18</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="19"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+        <v>17</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="28.8" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="14"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="28.8" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
+    <row r="10" spans="1:10" ht="28.8">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="6"/>
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
@@ -683,10 +700,10 @@
       <c r="F11" s="14"/>
       <c r="G11" s="9"/>
       <c r="J11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="9.75" customHeight="1">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -695,7 +712,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -704,7 +721,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="G14" s="2"/>
     </row>
   </sheetData>
@@ -732,24 +749,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>